<commit_message>
Added cover sheets and Config and Classification file
</commit_message>
<xml_diff>
--- a/RECC_Config_V2_0.xlsx
+++ b/RECC_Config_V2_0.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8544" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8544" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11176" uniqueCount="668">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11129" uniqueCount="680">
   <si>
     <t>User Name</t>
   </si>
@@ -2036,6 +2036,43 @@
   </si>
   <si>
     <t>3_MC_RECC_appliances</t>
+  </si>
+  <si>
+    <t>lifetime of EGT products in use phase</t>
+  </si>
+  <si>
+    <t>rgSR</t>
+  </si>
+  <si>
+    <t>RECC Cu status</t>
+  </si>
+  <si>
+    <t>2a33a77e-aed8-11e9-a2a3-2a2ae2dbcce4</t>
+  </si>
+  <si>
+    <t>2a33aa08-aed8-11e9-a2a3-2a2ae2dbcce4</t>
+  </si>
+  <si>
+    <t>2a33ab66-aed8-11e9-a2a3-2a2ae2dbcce4</t>
+  </si>
+  <si>
+    <t>2a33aca6-aed8-11e9-a2a3-2a2ae2dbcce4</t>
+  </si>
+  <si>
+    <t>2a33addc-aed8-11e9-a2a3-2a2ae2dbcce4</t>
+  </si>
+  <si>
+    <t>2a33b0fc-aed8-11e9-a2a3-2a2ae2dbcce4</t>
+  </si>
+  <si>
+    <t>2a33b32c-aed8-11e9-a2a3-2a2ae2dbcce4</t>
+  </si>
+  <si>
+    <t>2a33b48a-aed8-11e9-a2a3-2a2ae2dbcce4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+</t>
   </si>
 </sst>
 </file>
@@ -2339,7 +2376,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="95">
+  <cellXfs count="100">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2505,6 +2542,13 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -39255,7 +39299,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:Q136"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="C93" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
@@ -42565,8 +42609,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:Q144"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B39" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E94" sqref="E94"/>
+    <sheetView tabSelected="1" topLeftCell="A51" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="I85" sqref="I85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -42586,8 +42630,8 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B2" s="13" t="s">
-        <v>6</v>
+      <c r="B2" s="99" t="s">
+        <v>528</v>
       </c>
       <c r="C2" s="14"/>
       <c r="D2" s="14"/>
@@ -43714,7 +43758,7 @@
         <v>187</v>
       </c>
       <c r="L70" s="32" t="s">
-        <v>188</v>
+        <v>670</v>
       </c>
       <c r="M70" s="32" t="s">
         <v>189</v>
@@ -43731,7 +43775,7 @@
         <v>0</v>
       </c>
       <c r="B71" s="54" t="s">
-        <v>192</v>
+        <v>167</v>
       </c>
       <c r="C71" s="83" t="s">
         <v>661</v>
@@ -43740,34 +43784,21 @@
       <c r="E71" s="69" t="s">
         <v>528</v>
       </c>
-      <c r="F71" s="73" t="s">
-        <v>196</v>
-      </c>
-      <c r="G71" s="69" t="s">
-        <v>197</v>
-      </c>
-      <c r="H71" s="69" t="s">
-        <v>134</v>
-      </c>
+      <c r="G71" s="69"/>
+      <c r="H71" s="69"/>
       <c r="I71" t="s">
-        <v>198</v>
-      </c>
-      <c r="J71" t="s">
-        <v>199</v>
-      </c>
-      <c r="K71" s="36"/>
-      <c r="L71" t="s">
-        <v>200</v>
-      </c>
-      <c r="M71" t="s">
-        <v>201</v>
-      </c>
-      <c r="N71" s="51" t="s">
-        <v>202</v>
-      </c>
-      <c r="O71" t="s">
-        <v>203</v>
-      </c>
+        <v>672</v>
+      </c>
+      <c r="J71" s="41" t="s">
+        <v>209</v>
+      </c>
+      <c r="K71" s="42"/>
+      <c r="L71"/>
+      <c r="M71"/>
+      <c r="N71" s="95"/>
+      <c r="O71" s="95"/>
+      <c r="P71" s="95"/>
+      <c r="Q71" s="95"/>
     </row>
     <row r="72" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A72">
@@ -43785,34 +43816,21 @@
       <c r="E72" s="69" t="s">
         <v>528</v>
       </c>
-      <c r="F72" s="73" t="s">
-        <v>207</v>
-      </c>
-      <c r="G72" s="69" t="s">
-        <v>197</v>
-      </c>
-      <c r="H72" s="69" t="s">
-        <v>134</v>
-      </c>
+      <c r="G72" s="69"/>
+      <c r="H72" s="69"/>
       <c r="I72" t="s">
-        <v>208</v>
+        <v>673</v>
       </c>
       <c r="J72" t="s">
         <v>209</v>
       </c>
-      <c r="K72" s="36"/>
-      <c r="L72" t="s">
-        <v>210</v>
-      </c>
-      <c r="M72" t="s">
-        <v>211</v>
-      </c>
-      <c r="N72" s="49" t="s">
-        <v>212</v>
-      </c>
-      <c r="O72" t="s">
-        <v>213</v>
-      </c>
+      <c r="K72" s="42"/>
+      <c r="L72"/>
+      <c r="M72"/>
+      <c r="N72" s="95"/>
+      <c r="O72" s="95"/>
+      <c r="P72" s="95"/>
+      <c r="Q72" s="95"/>
     </row>
     <row r="73" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A73">
@@ -43825,39 +43843,26 @@
         <v>662</v>
       </c>
       <c r="D73" s="69" t="s">
-        <v>215</v>
+        <v>668</v>
       </c>
       <c r="E73" s="69" t="s">
         <v>528</v>
       </c>
-      <c r="F73" s="73" t="s">
-        <v>217</v>
-      </c>
-      <c r="G73" s="69" t="s">
-        <v>218</v>
-      </c>
-      <c r="H73" s="69" t="s">
-        <v>134</v>
-      </c>
+      <c r="G73" s="69"/>
+      <c r="H73" s="69"/>
       <c r="I73" s="63" t="s">
-        <v>219</v>
-      </c>
-      <c r="J73" t="s">
-        <v>199</v>
-      </c>
-      <c r="K73" s="36"/>
-      <c r="L73" t="s">
-        <v>210</v>
-      </c>
-      <c r="M73" t="s">
-        <v>220</v>
-      </c>
-      <c r="N73" s="51" t="s">
-        <v>221</v>
-      </c>
-      <c r="O73" t="s">
-        <v>222</v>
-      </c>
+        <v>674</v>
+      </c>
+      <c r="J73" s="41" t="s">
+        <v>209</v>
+      </c>
+      <c r="K73" s="42"/>
+      <c r="L73"/>
+      <c r="M73"/>
+      <c r="N73" s="95"/>
+      <c r="O73" s="95"/>
+      <c r="P73" s="95"/>
+      <c r="Q73" s="95"/>
     </row>
     <row r="74" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A74">
@@ -43875,34 +43880,21 @@
       <c r="E74" s="75" t="s">
         <v>528</v>
       </c>
-      <c r="F74" s="78" t="s">
-        <v>226</v>
-      </c>
-      <c r="G74" s="75" t="s">
-        <v>227</v>
-      </c>
-      <c r="H74" s="75" t="s">
-        <v>134</v>
-      </c>
-      <c r="I74" s="40" t="s">
-        <v>228</v>
-      </c>
-      <c r="J74" s="40" t="s">
-        <v>199</v>
-      </c>
-      <c r="K74" s="36"/>
-      <c r="L74" s="40" t="s">
-        <v>229</v>
-      </c>
-      <c r="M74" s="40" t="s">
-        <v>230</v>
-      </c>
-      <c r="N74" s="57" t="s">
-        <v>231</v>
-      </c>
-      <c r="O74" s="40" t="s">
-        <v>222</v>
-      </c>
+      <c r="G74" s="75"/>
+      <c r="H74" s="75"/>
+      <c r="I74" t="s">
+        <v>675</v>
+      </c>
+      <c r="J74" s="41" t="s">
+        <v>209</v>
+      </c>
+      <c r="K74" s="42"/>
+      <c r="L74" s="40"/>
+      <c r="M74" s="40"/>
+      <c r="N74" s="96"/>
+      <c r="O74" s="96"/>
+      <c r="P74" s="95"/>
+      <c r="Q74" s="95"/>
     </row>
     <row r="75" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A75">
@@ -43920,34 +43912,21 @@
       <c r="E75" s="69" t="s">
         <v>528</v>
       </c>
-      <c r="F75" s="76" t="s">
-        <v>235</v>
-      </c>
-      <c r="G75" s="69" t="s">
-        <v>197</v>
-      </c>
-      <c r="H75" s="69" t="s">
-        <v>134</v>
-      </c>
-      <c r="I75" t="s">
-        <v>236</v>
-      </c>
-      <c r="J75" t="s">
-        <v>199</v>
-      </c>
-      <c r="K75" s="36"/>
-      <c r="L75" t="s">
-        <v>210</v>
-      </c>
-      <c r="M75" t="s">
-        <v>237</v>
-      </c>
-      <c r="N75" s="51" t="s">
-        <v>238</v>
-      </c>
-      <c r="O75" t="s">
-        <v>222</v>
-      </c>
+      <c r="G75" s="69"/>
+      <c r="H75" s="69"/>
+      <c r="I75" s="41" t="s">
+        <v>676</v>
+      </c>
+      <c r="J75" s="41" t="s">
+        <v>209</v>
+      </c>
+      <c r="K75" s="35"/>
+      <c r="L75"/>
+      <c r="M75"/>
+      <c r="N75" s="95"/>
+      <c r="O75" s="95"/>
+      <c r="P75" s="95"/>
+      <c r="Q75" s="95"/>
     </row>
     <row r="76" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A76">
@@ -43965,34 +43944,21 @@
       <c r="E76" s="75" t="s">
         <v>528</v>
       </c>
-      <c r="F76" s="76" t="s">
-        <v>242</v>
-      </c>
-      <c r="G76" s="69" t="s">
-        <v>243</v>
-      </c>
-      <c r="H76" s="69" t="s">
-        <v>134</v>
-      </c>
+      <c r="G76" s="69"/>
+      <c r="H76" s="69"/>
       <c r="I76" t="s">
-        <v>244</v>
+        <v>677</v>
       </c>
       <c r="J76" t="s">
         <v>209</v>
       </c>
-      <c r="K76" s="42"/>
-      <c r="L76" t="s">
-        <v>245</v>
-      </c>
-      <c r="M76" t="s">
-        <v>246</v>
-      </c>
-      <c r="N76" s="51" t="s">
-        <v>247</v>
-      </c>
-      <c r="O76" t="s">
-        <v>222</v>
-      </c>
+      <c r="K76" s="35"/>
+      <c r="L76"/>
+      <c r="M76"/>
+      <c r="N76" s="95"/>
+      <c r="O76" s="95"/>
+      <c r="P76" s="95"/>
+      <c r="Q76" s="95"/>
     </row>
     <row r="77" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A77">
@@ -44010,34 +43976,21 @@
       <c r="E77" s="69" t="s">
         <v>528</v>
       </c>
-      <c r="F77" s="73" t="s">
-        <v>251</v>
-      </c>
-      <c r="G77" s="69" t="s">
-        <v>118</v>
-      </c>
-      <c r="H77" s="69" t="s">
-        <v>134</v>
-      </c>
+      <c r="G77" s="69"/>
+      <c r="H77" s="69"/>
       <c r="I77" t="s">
-        <v>252</v>
+        <v>678</v>
       </c>
       <c r="J77" t="s">
         <v>209</v>
       </c>
-      <c r="K77" s="36"/>
-      <c r="L77" t="s">
-        <v>210</v>
-      </c>
-      <c r="M77" t="s">
-        <v>253</v>
-      </c>
-      <c r="N77" s="49" t="s">
-        <v>254</v>
-      </c>
-      <c r="O77" t="s">
-        <v>213</v>
-      </c>
+      <c r="K77" s="35"/>
+      <c r="L77"/>
+      <c r="M77"/>
+      <c r="N77" s="95"/>
+      <c r="O77" s="95"/>
+      <c r="P77" s="95"/>
+      <c r="Q77" s="95"/>
     </row>
     <row r="78" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A78">
@@ -44055,36 +44008,21 @@
       <c r="E78" s="75" t="s">
         <v>528</v>
       </c>
-      <c r="F78" s="78" t="s">
-        <v>258</v>
-      </c>
-      <c r="G78" s="75" t="s">
-        <v>243</v>
-      </c>
-      <c r="H78" s="75" t="s">
-        <v>134</v>
-      </c>
-      <c r="I78" s="40" t="s">
-        <v>259</v>
+      <c r="G78" s="75"/>
+      <c r="H78" s="75"/>
+      <c r="I78" s="97" t="s">
+        <v>671</v>
       </c>
       <c r="J78" s="40" t="s">
         <v>209</v>
       </c>
-      <c r="K78" s="36"/>
-      <c r="L78" s="40" t="s">
-        <v>229</v>
-      </c>
-      <c r="M78" s="40" t="s">
-        <v>260</v>
-      </c>
-      <c r="N78" s="60" t="s">
-        <v>261</v>
-      </c>
-      <c r="O78" s="40" t="s">
-        <v>213</v>
-      </c>
-      <c r="P78" s="40"/>
-      <c r="Q78" s="40"/>
+      <c r="K78" s="35"/>
+      <c r="L78" s="40"/>
+      <c r="M78" s="40"/>
+      <c r="N78" s="96"/>
+      <c r="O78" s="96"/>
+      <c r="P78" s="96"/>
+      <c r="Q78" s="96"/>
     </row>
     <row r="79" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A79" s="85"/>
@@ -44225,7 +44163,9 @@
       <c r="C86" s="87"/>
       <c r="D86" s="85"/>
       <c r="E86" s="85"/>
-      <c r="F86" s="90"/>
+      <c r="F86" s="73" t="s">
+        <v>196</v>
+      </c>
       <c r="G86" s="85"/>
       <c r="H86" s="85"/>
       <c r="I86" s="92"/>
@@ -44244,7 +44184,9 @@
       <c r="C87" s="87"/>
       <c r="D87" s="85"/>
       <c r="E87" s="85"/>
-      <c r="F87" s="90"/>
+      <c r="F87" s="73" t="s">
+        <v>207</v>
+      </c>
       <c r="G87" s="85"/>
       <c r="H87" s="85"/>
       <c r="I87" s="85"/>
@@ -44263,7 +44205,9 @@
       <c r="C88" s="87"/>
       <c r="D88" s="85"/>
       <c r="E88" s="85"/>
-      <c r="F88" s="90"/>
+      <c r="F88" s="73" t="s">
+        <v>669</v>
+      </c>
       <c r="G88" s="85"/>
       <c r="H88" s="85"/>
       <c r="I88" s="85"/>
@@ -44282,7 +44226,9 @@
       <c r="C89" s="87"/>
       <c r="D89" s="85"/>
       <c r="E89" s="85"/>
-      <c r="F89" s="90"/>
+      <c r="F89" s="78" t="s">
+        <v>226</v>
+      </c>
       <c r="G89" s="85"/>
       <c r="H89" s="85"/>
       <c r="I89" s="85"/>
@@ -44295,16 +44241,20 @@
       <c r="P89" s="85"/>
       <c r="Q89" s="85"/>
     </row>
-    <row r="90" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:17" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A90" s="85"/>
       <c r="B90" s="89"/>
       <c r="C90" s="87"/>
       <c r="D90" s="85"/>
       <c r="E90" s="85"/>
-      <c r="F90" s="90"/>
+      <c r="F90" s="76" t="s">
+        <v>235</v>
+      </c>
       <c r="G90" s="85"/>
       <c r="H90" s="85"/>
-      <c r="I90" s="85"/>
+      <c r="I90" s="98" t="s">
+        <v>679</v>
+      </c>
       <c r="J90" s="85"/>
       <c r="K90" s="85"/>
       <c r="L90" s="85"/>
@@ -44320,7 +44270,9 @@
       <c r="C91" s="87"/>
       <c r="D91" s="85"/>
       <c r="E91" s="87"/>
-      <c r="F91" s="90"/>
+      <c r="F91" s="76" t="s">
+        <v>242</v>
+      </c>
       <c r="G91" s="85"/>
       <c r="H91" s="85"/>
       <c r="I91" s="85"/>
@@ -44339,7 +44291,9 @@
       <c r="C92" s="87"/>
       <c r="D92" s="85"/>
       <c r="E92" s="87"/>
-      <c r="F92" s="90"/>
+      <c r="F92" s="73" t="s">
+        <v>669</v>
+      </c>
       <c r="G92" s="85"/>
       <c r="H92" s="85"/>
       <c r="I92" s="85"/>
@@ -44358,7 +44312,9 @@
       <c r="C93" s="87"/>
       <c r="D93" s="85"/>
       <c r="E93" s="85"/>
-      <c r="F93" s="90"/>
+      <c r="F93" s="78" t="s">
+        <v>258</v>
+      </c>
       <c r="G93" s="85"/>
       <c r="H93" s="85"/>
       <c r="I93" s="85"/>

</xml_diff>

<commit_message>
Adding Index Structure to config file and saving new RECC_G71C
</commit_message>
<xml_diff>
--- a/RECC_Config_V2_0.xlsx
+++ b/RECC_Config_V2_0.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8544" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8544" firstSheet="1" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11129" uniqueCount="680">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11133" uniqueCount="682">
   <si>
     <t>User Name</t>
   </si>
@@ -2073,6 +2073,12 @@
   <si>
     <t xml:space="preserve">
 </t>
+  </si>
+  <si>
+    <t>rSRGt</t>
+  </si>
+  <si>
+    <t>rSRG</t>
   </si>
 </sst>
 </file>
@@ -3014,8 +3020,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:Q136"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView topLeftCell="C70" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -39299,8 +39305,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:Q136"/>
   <sheetViews>
-    <sheetView topLeftCell="C93" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView topLeftCell="C60" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F65" sqref="F65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -42609,8 +42615,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:Q144"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="I85" sqref="I85"/>
+    <sheetView tabSelected="1" topLeftCell="C54" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F77" sqref="F77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -43784,6 +43790,9 @@
       <c r="E71" s="69" t="s">
         <v>528</v>
       </c>
+      <c r="F71" s="90" t="s">
+        <v>680</v>
+      </c>
       <c r="G71" s="69"/>
       <c r="H71" s="69"/>
       <c r="I71" t="s">
@@ -43816,6 +43825,9 @@
       <c r="E72" s="69" t="s">
         <v>528</v>
       </c>
+      <c r="F72" s="90" t="s">
+        <v>680</v>
+      </c>
       <c r="G72" s="69"/>
       <c r="H72" s="69"/>
       <c r="I72" t="s">
@@ -43848,6 +43860,9 @@
       <c r="E73" s="69" t="s">
         <v>528</v>
       </c>
+      <c r="F73" s="90" t="s">
+        <v>681</v>
+      </c>
       <c r="G73" s="69"/>
       <c r="H73" s="69"/>
       <c r="I73" s="63" t="s">
@@ -43879,6 +43894,9 @@
       </c>
       <c r="E74" s="75" t="s">
         <v>528</v>
+      </c>
+      <c r="F74" s="90" t="s">
+        <v>681</v>
       </c>
       <c r="G74" s="75"/>
       <c r="H74" s="75"/>

</xml_diff>

<commit_message>
Adding input for dsm for indurstry in RECC_G7IC_V2_0
</commit_message>
<xml_diff>
--- a/RECC_Config_V2_0.xlsx
+++ b/RECC_Config_V2_0.xlsx
@@ -3087,8 +3087,8 @@
   </sheetPr>
   <dimension ref="A2:Q150"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G52" sqref="G52"/>
+    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C73" sqref="C73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>